<commit_message>
Add in multiple scopes, country and region
</commit_message>
<xml_diff>
--- a/tests/integration_test_files/scope_1.xlsx
+++ b/tests/integration_test_files/scope_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm/tests/integration_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65CCD0F0-654C-9F4A-BB99-410238A4AC2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A779D0E-5F43-6F4B-8B03-8A919909C59B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="64600" yWindow="4160" windowWidth="33600" windowHeight="19480" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="571">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="573">
   <si>
     <t>Epoch</t>
   </si>
@@ -1779,12 +1779,6 @@
     <t>Protocol Approval</t>
   </si>
   <si>
-    <t>scope</t>
-  </si>
-  <si>
-    <t>GLOBAL</t>
-  </si>
-  <si>
     <t>Sponsor Approval Date</t>
   </si>
   <si>
@@ -1792,6 +1786,18 @@
   </si>
   <si>
     <t>SCOPE1</t>
+  </si>
+  <si>
+    <t>country: GBR, country:FRA</t>
+  </si>
+  <si>
+    <t>region:asia</t>
+  </si>
+  <si>
+    <t>region: europe</t>
+  </si>
+  <si>
+    <t>scopes</t>
   </si>
 </sst>
 </file>
@@ -2274,10 +2280,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53AA772F-4124-4842-BA10-D27E5C5CE960}">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2287,6 +2293,7 @@
     <col min="3" max="3" width="32.83203125" customWidth="1"/>
     <col min="4" max="4" width="24.6640625" customWidth="1"/>
     <col min="5" max="6" width="24.6640625" style="26" customWidth="1"/>
+    <col min="7" max="7" width="34.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -2294,7 +2301,7 @@
         <v>484</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -2421,7 +2428,7 @@
         <v>558</v>
       </c>
       <c r="G16" s="19" t="s">
-        <v>566</v>
+        <v>572</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -2438,13 +2445,13 @@
         <v>562</v>
       </c>
       <c r="E17" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="F17" s="31">
         <v>44927</v>
       </c>
       <c r="G17" t="s">
-        <v>567</v>
+        <v>569</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -2461,13 +2468,36 @@
         <v>565</v>
       </c>
       <c r="E18" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="F18" s="31">
         <v>44927</v>
       </c>
       <c r="G18" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="11" t="s">
+        <v>563</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>560</v>
+      </c>
+      <c r="C19" t="s">
+        <v>564</v>
+      </c>
+      <c r="D19" t="s">
+        <v>565</v>
+      </c>
+      <c r="E19" t="s">
         <v>567</v>
+      </c>
+      <c r="F19" s="31">
+        <v>44958</v>
+      </c>
+      <c r="G19" t="s">
+        <v>570</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Amed syntax from ':' to '=' for scopes
</commit_message>
<xml_diff>
--- a/tests/integration_test_files/scope_1.xlsx
+++ b/tests/integration_test_files/scope_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm/tests/integration_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A779D0E-5F43-6F4B-8B03-8A919909C59B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8361D8B3-41A0-F74B-8537-007CB5465AD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="64600" yWindow="4160" windowWidth="33600" windowHeight="19480" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
@@ -1770,6 +1770,9 @@
     <t>Design Approval</t>
   </si>
   <si>
+    <t>Global</t>
+  </si>
+  <si>
     <t>protocol_document</t>
   </si>
   <si>
@@ -1788,16 +1791,13 @@
     <t>SCOPE1</t>
   </si>
   <si>
-    <t>country: GBR, country:FRA</t>
-  </si>
-  <si>
     <t>region:asia</t>
   </si>
   <si>
-    <t>region: europe</t>
-  </si>
-  <si>
     <t>scopes</t>
+  </si>
+  <si>
+    <t>country = GBR, country=FRA, region=ASIA, country=USA</t>
   </si>
 </sst>
 </file>
@@ -2283,7 +2283,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2293,7 +2293,7 @@
     <col min="3" max="3" width="32.83203125" customWidth="1"/>
     <col min="4" max="4" width="24.6640625" customWidth="1"/>
     <col min="5" max="6" width="24.6640625" style="26" customWidth="1"/>
-    <col min="7" max="7" width="34.5" customWidth="1"/>
+    <col min="7" max="7" width="47.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -2301,7 +2301,7 @@
         <v>484</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -2428,7 +2428,7 @@
         <v>558</v>
       </c>
       <c r="G16" s="19" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -2445,53 +2445,53 @@
         <v>562</v>
       </c>
       <c r="E17" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="F17" s="31">
         <v>44927</v>
       </c>
       <c r="G17" t="s">
-        <v>569</v>
+        <v>572</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="11" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="B18" s="11" t="s">
         <v>560</v>
       </c>
       <c r="C18" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="D18" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="E18" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="F18" s="31">
         <v>44927</v>
       </c>
       <c r="G18" t="s">
-        <v>571</v>
+        <v>563</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="11" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="B19" s="11" t="s">
         <v>560</v>
       </c>
       <c r="C19" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="D19" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="E19" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="F19" s="31">
         <v>44958</v>

</xml_diff>

<commit_message>
Further XL sheet changes
</commit_message>
<xml_diff>
--- a/tests/integration_test_files/scope_1.xlsx
+++ b/tests/integration_test_files/scope_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm/tests/integration_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76A72130-6B83-0640-9022-0FD45253125F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{579B710B-0D03-694D-AF8A-B72F5DA4D734}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="64600" yWindow="4160" windowWidth="33600" windowHeight="19480" firstSheet="4" activeTab="11" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="27840" yWindow="500" windowWidth="33600" windowHeight="19480" firstSheet="4" activeTab="5" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="800" uniqueCount="638">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="798" uniqueCount="638">
   <si>
     <t>Screening</t>
   </si>
@@ -2160,10 +2160,10 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2859,7 +2859,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B908C5D6-C6A1-4043-A49A-69C599CFBAE9}">
   <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="E2" sqref="E2:E3"/>
     </sheetView>
   </sheetViews>
@@ -5315,34 +5315,34 @@
       <c r="A3" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="31" t="s">
         <v>139</v>
       </c>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="30" t="s">
         <v>159</v>
       </c>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="31" t="s">
+      <c r="B5" s="30" t="s">
         <v>123</v>
       </c>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="15" t="s">
@@ -5462,16 +5462,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="B10:E10"/>
     <mergeCell ref="B8:E8"/>
     <mergeCell ref="B4:E4"/>
     <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5632,11 +5632,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{136502A0-3DDE-CC47-9DA7-EB2F3073B24B}">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane xSplit="3" ySplit="9" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="B19" sqref="B19"/>
+      <selection pane="bottomRight" activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5835,9 +5835,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="A10" s="2"/>
       <c r="B10" s="3" t="s">
         <v>5</v>
       </c>
@@ -5861,9 +5859,7 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="A11" s="2"/>
       <c r="B11" s="4" t="s">
         <v>12</v>
       </c>

</xml_diff>